<commit_message>
rebuild cleanly with lowercase exercise
</commit_message>
<xml_diff>
--- a/ids541_specific/class_schedule_541_xlsx.xlsx
+++ b/ids541_specific/class_schedule_541_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids541_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B2B5EB-1362-CC4F-9FC3-67294D8E3CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E7EFBC-D861-3841-8253-3479FA2DED58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17780" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Topic</t>
   </si>
@@ -59,9 +59,6 @@
 - `Parquet Format &lt;../notebooks/PDS_not_yet_in_coursera/30_big_data/30_parquet.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Link &lt;exercises/Exercise_bigdata.html&gt;`_</t>
-  </si>
-  <si>
     <t>- Parallelism 
 - Distributed Computing</t>
   </si>
@@ -72,10 +69,6 @@
 (Note reading includes a 45 minute video to watch)</t>
   </si>
   <si>
-    <t>- `Dask &lt;exercises/Exercise_dask_realdata.html&gt;`_
-- `More dask (optional) &lt;exercises/Exercise_dask.html&gt;`_</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -161,13 +154,6 @@
 - `Solving Performance Problems &lt;../notebooks/PDS_not_yet_in_coursera/30_big_data/50_performance_solutions.html&gt;`_</t>
   </si>
   <si>
-    <t>- Raster Data
-- Intro to Rasterio</t>
-  </si>
-  <si>
-    <t>- Remote Sensing and Satellite Data</t>
-  </si>
-  <si>
     <t>- Network Data</t>
   </si>
   <si>
@@ -181,15 +167,6 @@
   </si>
   <si>
     <t>**NO CLASS**</t>
-  </si>
-  <si>
-    <t>- NLP</t>
-  </si>
-  <si>
-    <t>- Advanced Modelling</t>
-  </si>
-  <si>
-    <t>- Larger Programs</t>
   </si>
   <si>
     <t>- SciKit-Learn</t>
@@ -204,12 +181,6 @@
 - `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_</t>
   </si>
   <si>
-    <t>- `Link &lt;../ids720_specific/exercises/Exercise_reshaping.html&gt;`_</t>
-  </si>
-  <si>
-    <t>- GIS</t>
-  </si>
-  <si>
     <t>- Supervised ML</t>
   </si>
   <si>
@@ -238,13 +209,59 @@
   </si>
   <si>
     <t>- `Mapping &lt;../notebooks/gis/25_gis_mapping.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;../ids720_specific/exercises/exercise_reshaping.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link &lt;exercises/exercise_bigdata.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Dask &lt;exercises/exercise_dask_realdata.html&gt;`_
+- `More dask (optional) &lt;exercises/exercise_dask.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Raster Data
+- Intro to Rasterio and X-Array</t>
+  </si>
+  <si>
+    <t>- Plotting raster data</t>
+  </si>
+  <si>
+    <t>- Remote Sensing and Satellite Data
+- Band Algebra</t>
+  </si>
+  <si>
+    <t>- Reprojection, resampling, and interpolation</t>
+  </si>
+  <si>
+    <t>- GIS: Mixing Vector and Raster</t>
+  </si>
+  <si>
+    <t>- Zonal aggregation (summary statistics)
+- Rasterization/Geohashing</t>
+  </si>
+  <si>
+    <t>- GIS: Rasters</t>
+  </si>
+  <si>
+    <t>-GIS: Vector Data</t>
+  </si>
+  <si>
+    <t>- Solving Problems with Data</t>
+  </si>
+  <si>
+    <t>- `Solving Problems with Data &lt;https://ds4humans.com/10_introduction/10_solving_problems_with_data.html&gt;`_</t>
+  </si>
+  <si>
+    <t>- Problem Taxonomy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -272,6 +289,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1F2328"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -314,10 +337,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,7 +669,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -661,27 +683,27 @@
     </row>
     <row r="2" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
@@ -690,7 +712,7 @@
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
@@ -699,261 +721,262 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" s="9" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="10"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="7"/>
+        <v>41</v>
+      </c>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -963,7 +986,7 @@
       <c r="C29" s="9"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
+      <c r="A32" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update elective requirement and schedules
</commit_message>
<xml_diff>
--- a/ids541_specific/class_schedule_541_xlsx.xlsx
+++ b/ids541_specific/class_schedule_541_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nce8/github/practicaldatascience_book/ids541_specific/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2DEDA9-9FEF-6D42-B087-BB7F4122954A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAE7169-022A-BF45-AEA0-2383E30AEA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>Topic</t>
   </si>
@@ -255,6 +255,9 @@
   <si>
     <t>- Géron, Chpt 1: The Machine Learning Landscape (stop before "Batch and Online Learning," then read the "Testing and Validating" section)
 - Géron, Chpt 2: End-to-End Machine Learning Project</t>
+  </si>
+  <si>
+    <t>- Working with Text</t>
   </si>
 </sst>
 </file>
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,40 +710,44 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="2"/>
-      <c r="C4" s="7"/>
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>54</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>62</v>
@@ -752,7 +759,7 @@
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>62</v>
@@ -764,7 +771,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>62</v>
@@ -775,7 +782,7 @@
     </row>
     <row r="10" spans="1:4" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>62</v>
@@ -787,7 +794,7 @@
     </row>
     <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>61</v>
@@ -799,7 +806,7 @@
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>61</v>
@@ -811,7 +818,7 @@
     </row>
     <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>61</v>
@@ -822,7 +829,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>61</v>
@@ -833,7 +840,7 @@
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>59</v>
@@ -844,7 +851,7 @@
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>46</v>
@@ -856,7 +863,7 @@
     </row>
     <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>46</v>
@@ -867,7 +874,7 @@
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>46</v>
@@ -879,7 +886,7 @@
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>46</v>
@@ -890,7 +897,7 @@
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>63</v>
@@ -901,7 +908,7 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>63</v>
@@ -912,7 +919,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>41</v>
@@ -920,7 +927,7 @@
     </row>
     <row r="23" spans="1:4" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>41</v>
@@ -929,7 +936,7 @@
     </row>
     <row r="24" spans="1:4" ht="140" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>63</v>
@@ -938,51 +945,45 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>63</v>
+        <v>37</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" ht="134" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>40</v>
+      <c r="B28" t="s">
+        <v>5</v>
       </c>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
       <c r="C29" s="9"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>